<commit_message>
Small corrections to harmonize the models
</commit_message>
<xml_diff>
--- a/Matlab/Model/Model_Akt/SBTAB_akt_Original_Paper.xlsx
+++ b/Matlab/Model/Model_Akt/SBTAB_akt_Original_Paper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Akt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AFC209-4E77-4142-B1AD-628224457B1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFC77B5-6EB4-4DF6-97FB-A12FA9DC06D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="26700" windowWidth="29040" windowHeight="15840" tabRatio="857" firstSheet="9" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="27015" windowWidth="29040" windowHeight="15840" tabRatio="857" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compound" sheetId="4" r:id="rId1"/>
@@ -1063,10 +1063,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1479,17 +1479,17 @@
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:27" ht="13.5">
@@ -11561,7 +11561,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11617,7 +11617,7 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="27" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -21162,11 +21162,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B3:B16"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21961,7 +21961,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>9.0092383313698996E-5</v>
       </c>
       <c r="H4">
@@ -23754,7 +23754,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>2.6076863961724901E-4</v>
       </c>
       <c r="H4">
@@ -25547,7 +25547,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>7.74295778326481E-4</v>
       </c>
       <c r="H4">
@@ -27340,7 +27340,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>1.7761848137009401E-3</v>
       </c>
       <c r="H4">
@@ -29133,7 +29133,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>3.2994828878185698E-3</v>
       </c>
       <c r="H4">
@@ -31753,7 +31753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD873178-5B7B-4239-8036-3F423BECD543}">
   <dimension ref="A1:AE103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -31878,7 +31878,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <v>4.4824817429268997E-3</v>
       </c>
       <c r="H4">

</xml_diff>

<commit_message>
Reformated units on models parameters
</commit_message>
<xml_diff>
--- a/Matlab/Model/Model_Akt/SBTAB_akt_Original_Paper.xlsx
+++ b/Matlab/Model/Model_Akt/SBTAB_akt_Original_Paper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Akt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E53693-2566-4034-B02A-67504292F09E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F9BEC1-EDDD-4837-B36A-623C5D547135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" tabRatio="857" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" tabRatio="857" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compound" sheetId="4" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <sheet name="E17" sheetId="69" r:id="rId40"/>
     <sheet name="E17I" sheetId="70" r:id="rId41"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>Experiment 1</t>
-  </si>
-  <si>
-    <t>1/(nanomolarity*second)</t>
   </si>
   <si>
     <t>K1</t>
@@ -890,6 +887,9 @@
   <si>
     <t>Experiment 18</t>
   </si>
+  <si>
+    <t>liter/(nanomole*second)</t>
+  </si>
 </sst>
 </file>
 
@@ -1509,10 +1509,10 @@
         <v>21</v>
       </c>
       <c r="F2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>79</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>80</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>22</v>
@@ -1530,7 +1530,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>68</v>
@@ -1554,10 +1554,10 @@
         <v>25</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O3" s="26"/>
     </row>
@@ -1566,7 +1566,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>68</v>
@@ -1590,10 +1590,10 @@
         <v>25</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O4" s="26"/>
     </row>
@@ -1602,7 +1602,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>68</v>
@@ -1626,10 +1626,10 @@
         <v>25</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O5" s="26"/>
     </row>
@@ -1638,7 +1638,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>68</v>
@@ -1662,10 +1662,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O6" s="26"/>
     </row>
@@ -1674,7 +1674,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>68</v>
@@ -1698,10 +1698,10 @@
         <v>25</v>
       </c>
       <c r="I7" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="K7" s="32"/>
       <c r="L7" s="32"/>
@@ -1723,10 +1723,10 @@
     </row>
     <row r="8" spans="1:27" ht="14.25">
       <c r="A8" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>68</v>
@@ -1750,19 +1750,19 @@
         <v>25</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O8" s="26"/>
     </row>
     <row r="9" spans="1:27" ht="14.25">
       <c r="A9" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>96</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>97</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>68</v>
@@ -1786,19 +1786,19 @@
         <v>25</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J9" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O9" s="26"/>
     </row>
     <row r="10" spans="1:27" ht="14.25">
       <c r="A10" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>68</v>
@@ -1822,19 +1822,19 @@
         <v>25</v>
       </c>
       <c r="I10" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O10" s="26"/>
     </row>
     <row r="11" spans="1:27" ht="14.25">
       <c r="A11" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>68</v>
@@ -1858,19 +1858,19 @@
         <v>25</v>
       </c>
       <c r="I11" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O11" s="26"/>
     </row>
     <row r="12" spans="1:27" ht="14.25">
       <c r="A12" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>68</v>
@@ -1879,10 +1879,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G12" s="26" t="b">
         <f>FALSE()</f>
@@ -1892,19 +1892,19 @@
         <v>25</v>
       </c>
       <c r="I12" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>104</v>
       </c>
       <c r="O12" s="26"/>
     </row>
     <row r="13" spans="1:27" ht="14.25">
       <c r="A13" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>68</v>
@@ -1913,10 +1913,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G13" s="26" t="b">
         <f>FALSE()</f>
@@ -1926,10 +1926,10 @@
         <v>25</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O13" s="26"/>
     </row>
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -2633,10 +2633,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -3634,15 +3634,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -4426,10 +4426,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5427,15 +5427,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -6196,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -6219,10 +6219,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -7220,15 +7220,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -7989,7 +7989,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -8012,10 +8012,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -9013,15 +9013,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -9782,7 +9782,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -9805,10 +9805,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -10806,15 +10806,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -11658,17 +11658,17 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -11699,17 +11699,17 @@
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -11740,17 +11740,17 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -11781,17 +11781,17 @@
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -11816,23 +11816,23 @@
     </row>
     <row r="7" spans="1:26" ht="13.5">
       <c r="A7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -11857,23 +11857,23 @@
     </row>
     <row r="8" spans="1:26" ht="13.5">
       <c r="A8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -11898,23 +11898,23 @@
     </row>
     <row r="9" spans="1:26" ht="13.5">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -11939,23 +11939,23 @@
     </row>
     <row r="10" spans="1:26" ht="13.5">
       <c r="A10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -11980,23 +11980,23 @@
     </row>
     <row r="11" spans="1:26" ht="13.5">
       <c r="A11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D11" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -12021,23 +12021,23 @@
     </row>
     <row r="12" spans="1:26" ht="13.5">
       <c r="A12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -12062,23 +12062,23 @@
     </row>
     <row r="13" spans="1:26" ht="13.5">
       <c r="A13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -12215,7 +12215,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -12238,10 +12238,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -13239,15 +13239,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -14008,7 +14008,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -14031,10 +14031,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -15032,15 +15032,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -15801,7 +15801,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -15824,10 +15824,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -16825,15 +16825,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -17594,7 +17594,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -17617,10 +17617,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -18618,15 +18618,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -19387,7 +19387,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -19410,10 +19410,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -20411,15 +20411,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -21162,11 +21162,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21250,10 +21250,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>70</v>
+        <v>271</v>
       </c>
       <c r="E3" s="25">
         <f t="shared" ref="E3:E16" si="0">10^F3</f>
@@ -21263,10 +21263,10 @@
         <v>-2.1714586807558929</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="10"/>
@@ -21281,13 +21281,13 @@
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" s="25">
         <f t="shared" si="0"/>
@@ -21297,10 +21297,10 @@
         <v>-1.3898830445880721</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="10"/>
@@ -21315,13 +21315,13 @@
     </row>
     <row r="5" spans="1:19" ht="14.25">
       <c r="A5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>70</v>
+        <v>271</v>
       </c>
       <c r="E5" s="25">
         <f t="shared" si="0"/>
@@ -21331,10 +21331,10 @@
         <v>-4.8084651529932163</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="10"/>
@@ -21349,13 +21349,13 @@
     </row>
     <row r="6" spans="1:19" ht="14.25">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" s="25">
         <f t="shared" si="0"/>
@@ -21365,10 +21365,10 @@
         <v>-2.2861123053046994</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="10"/>
@@ -21383,13 +21383,13 @@
     </row>
     <row r="7" spans="1:19" ht="12.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E7" s="25">
         <f t="shared" si="0"/>
@@ -21399,10 +21399,10 @@
         <v>-1.5147272923617776</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="10"/>
@@ -21417,13 +21417,13 @@
     </row>
     <row r="8" spans="1:19" ht="14.25">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" s="25">
         <f t="shared" si="0"/>
@@ -21433,10 +21433,10 @@
         <v>-1.0012203432596507</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="10"/>
@@ -21451,13 +21451,13 @@
     </row>
     <row r="9" spans="1:19" ht="14.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>70</v>
+        <v>271</v>
       </c>
       <c r="E9" s="25">
         <f t="shared" si="0"/>
@@ -21467,10 +21467,10 @@
         <v>-5.6773900160161705</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="10"/>
@@ -21485,13 +21485,13 @@
     </row>
     <row r="10" spans="1:19" ht="14.25">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E10" s="25">
         <f t="shared" si="0"/>
@@ -21501,10 +21501,10 @@
         <v>-14.285720547548516</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="10"/>
@@ -21519,13 +21519,13 @@
     </row>
     <row r="11" spans="1:19" ht="14.25">
       <c r="A11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="0"/>
@@ -21535,10 +21535,10 @@
         <v>-2.9154308710048689</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="10"/>
@@ -21553,13 +21553,13 @@
     </row>
     <row r="12" spans="1:19" ht="14.25">
       <c r="A12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="25">
         <f t="shared" si="0"/>
@@ -21569,10 +21569,10 @@
         <v>-1.4841764738077223</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="10"/>
@@ -21587,13 +21587,13 @@
     </row>
     <row r="13" spans="1:19" ht="14.25">
       <c r="A13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="25">
         <f>10^F13</f>
@@ -21603,10 +21603,10 @@
         <v>-2.9465297153107599</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="10"/>
@@ -21621,13 +21621,13 @@
     </row>
     <row r="14" spans="1:19" ht="14.25">
       <c r="A14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14" s="25">
         <f t="shared" si="0"/>
@@ -21637,10 +21637,10 @@
         <v>-1.7158152480038114</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="10"/>
@@ -21655,13 +21655,13 @@
     </row>
     <row r="15" spans="1:19" ht="14.25">
       <c r="A15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E15" s="25">
         <f t="shared" si="0"/>
@@ -21671,10 +21671,10 @@
         <v>-3.9731155198115515</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="10"/>
@@ -21689,13 +21689,13 @@
     </row>
     <row r="16" spans="1:19" ht="14.25">
       <c r="A16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E16" s="25">
         <f t="shared" si="0"/>
@@ -21705,10 +21705,10 @@
         <v>-3.9731155198115515</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="10"/>
@@ -21854,7 +21854,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -21877,10 +21877,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -22878,15 +22878,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -23647,7 +23647,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -23670,10 +23670,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -24671,15 +24671,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -25440,7 +25440,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -25463,10 +25463,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -26464,15 +26464,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -27233,7 +27233,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -27256,10 +27256,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -28257,15 +28257,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -29026,7 +29026,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -29049,10 +29049,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -30050,15 +30050,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -30921,10 +30921,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D3" s="18" t="str">
         <f>_xlfn.CONCAT("SD_",A3)</f>
@@ -30944,10 +30944,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="16"/>
@@ -30976,10 +30976,10 @@
         <v>41</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="18" t="str">
         <f t="shared" ref="D4:D16" si="0">_xlfn.CONCAT("SD_",A4)</f>
@@ -30999,10 +30999,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="18"/>
@@ -31029,13 +31029,13 @@
     </row>
     <row r="5" spans="1:32" ht="14.25">
       <c r="A5" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D5" s="18" t="str">
         <f t="shared" si="0"/>
@@ -31055,10 +31055,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" s="18"/>
@@ -31085,10 +31085,10 @@
     </row>
     <row r="6" spans="1:32" ht="14.25">
       <c r="A6" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -31108,10 +31108,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
@@ -31138,10 +31138,10 @@
     </row>
     <row r="7" spans="1:32" ht="14.25">
       <c r="A7" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -31161,10 +31161,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -31191,10 +31191,10 @@
     </row>
     <row r="8" spans="1:32" ht="14.25">
       <c r="A8" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -31214,10 +31214,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
@@ -31244,10 +31244,10 @@
     </row>
     <row r="9" spans="1:32" ht="14.25">
       <c r="A9" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18" t="str">
@@ -31268,10 +31268,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
@@ -31298,10 +31298,10 @@
     </row>
     <row r="10" spans="1:32" ht="14.25">
       <c r="A10" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18" t="str">
@@ -31322,10 +31322,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
@@ -31352,10 +31352,10 @@
     </row>
     <row r="11" spans="1:32" ht="14.25">
       <c r="A11" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="str">
@@ -31376,10 +31376,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
@@ -31406,10 +31406,10 @@
     </row>
     <row r="12" spans="1:32" ht="14.25">
       <c r="A12" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="str">
@@ -31430,10 +31430,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
@@ -31460,10 +31460,10 @@
     </row>
     <row r="13" spans="1:32" ht="14.25">
       <c r="A13" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18" t="str">
@@ -31484,10 +31484,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -31514,10 +31514,10 @@
     </row>
     <row r="14" spans="1:32" ht="14.25">
       <c r="A14" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="18" t="str">
@@ -31538,10 +31538,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -31568,10 +31568,10 @@
     </row>
     <row r="15" spans="1:32" ht="14.25">
       <c r="A15" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="18" t="str">
@@ -31592,10 +31592,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
@@ -31622,10 +31622,10 @@
     </row>
     <row r="16" spans="1:32" ht="14.25">
       <c r="A16" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>203</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>204</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="str">
@@ -31646,10 +31646,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -31771,7 +31771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -31794,10 +31794,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -32795,15 +32795,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -33546,7 +33546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -33625,19 +33625,19 @@
         <v>46</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>164</v>
-      </c>
       <c r="J2" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>23</v>
@@ -33675,7 +33675,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>50</v>
@@ -33696,7 +33696,7 @@
         <v>68190.2</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M3" s="18">
         <v>-120</v>
@@ -33722,17 +33722,17 @@
     </row>
     <row r="4" spans="1:26" ht="14.25">
       <c r="A4" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>50</v>
@@ -33753,7 +33753,7 @@
         <v>68190.2</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M4" s="18">
         <v>-120</v>
@@ -33779,17 +33779,17 @@
     </row>
     <row r="5" spans="1:26" ht="14.25">
       <c r="A5" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>89</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>90</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>50</v>
@@ -33810,7 +33810,7 @@
         <v>68190.2</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M5" s="18">
         <v>-120</v>
@@ -33836,17 +33836,17 @@
     </row>
     <row r="6" spans="1:26" ht="14.25">
       <c r="A6" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>214</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>50</v>
@@ -33867,7 +33867,7 @@
         <v>68190.2</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M6" s="18">
         <v>-120</v>
@@ -33893,17 +33893,17 @@
     </row>
     <row r="7" spans="1:26" ht="14.25">
       <c r="A7" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>218</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>219</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>50</v>
@@ -33924,7 +33924,7 @@
         <v>68190.2</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M7" s="18">
         <v>-120</v>
@@ -33950,17 +33950,17 @@
     </row>
     <row r="8" spans="1:26" ht="14.25">
       <c r="A8" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>220</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>221</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>50</v>
@@ -33981,7 +33981,7 @@
         <v>68190.2</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M8" s="18">
         <v>-120</v>
@@ -34007,17 +34007,17 @@
     </row>
     <row r="9" spans="1:26" ht="14.25">
       <c r="A9" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>236</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>237</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>50</v>
@@ -34038,7 +34038,7 @@
         <v>68190.2</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M9" s="18">
         <v>-120</v>
@@ -34064,17 +34064,17 @@
     </row>
     <row r="10" spans="1:26" ht="14.25">
       <c r="A10" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>238</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>239</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>50</v>
@@ -34095,7 +34095,7 @@
         <v>68190.2</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M10" s="18">
         <v>-120</v>
@@ -34121,17 +34121,17 @@
     </row>
     <row r="11" spans="1:26" ht="14.25">
       <c r="A11" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>240</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>241</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>50</v>
@@ -34152,7 +34152,7 @@
         <v>68190.2</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M11" s="18">
         <v>-120</v>
@@ -34178,17 +34178,17 @@
     </row>
     <row r="12" spans="1:26" ht="14.25">
       <c r="A12" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>242</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>243</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>50</v>
@@ -34209,7 +34209,7 @@
         <v>68190.2</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M12" s="18">
         <v>-120</v>
@@ -34235,17 +34235,17 @@
     </row>
     <row r="13" spans="1:26" ht="14.25">
       <c r="A13" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>244</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>245</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>50</v>
@@ -34266,7 +34266,7 @@
         <v>68190.2</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M13" s="18">
         <v>-120</v>
@@ -34292,17 +34292,17 @@
     </row>
     <row r="14" spans="1:26" ht="14.25">
       <c r="A14" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>246</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>247</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>50</v>
@@ -34323,7 +34323,7 @@
         <v>68190.2</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M14" s="18">
         <v>-120</v>
@@ -34349,17 +34349,17 @@
     </row>
     <row r="15" spans="1:26" ht="14.25">
       <c r="A15" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>248</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>249</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>50</v>
@@ -34380,7 +34380,7 @@
         <v>68190.2</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M15" s="18">
         <v>-120</v>
@@ -34406,17 +34406,17 @@
     </row>
     <row r="16" spans="1:26" ht="14.25">
       <c r="A16" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>262</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>263</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>50</v>
@@ -34437,7 +34437,7 @@
         <v>68190.2</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M16" s="18">
         <v>-120</v>
@@ -34463,17 +34463,17 @@
     </row>
     <row r="17" spans="1:26" ht="14.25">
       <c r="A17" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>264</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>265</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>50</v>
@@ -34494,7 +34494,7 @@
         <v>68190.2</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M17" s="18">
         <v>-120</v>
@@ -34520,17 +34520,17 @@
     </row>
     <row r="18" spans="1:26" ht="14.25">
       <c r="A18" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>266</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>267</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>50</v>
@@ -34551,7 +34551,7 @@
         <v>68190.2</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M18" s="18">
         <v>-120</v>
@@ -34577,17 +34577,17 @@
     </row>
     <row r="19" spans="1:26" ht="14.25">
       <c r="A19" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>268</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>269</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>50</v>
@@ -34608,7 +34608,7 @@
         <v>68190.2</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M19" s="18">
         <v>-120</v>
@@ -34634,17 +34634,17 @@
     </row>
     <row r="20" spans="1:26" ht="14.25">
       <c r="A20" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>270</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>271</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>50</v>
@@ -34665,7 +34665,7 @@
         <v>68190.2</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M20" s="18">
         <v>-120</v>
@@ -35430,7 +35430,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -35453,10 +35453,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -36463,15 +36463,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>
@@ -37232,7 +37232,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -37255,10 +37255,10 @@
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -38256,15 +38256,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>57</v>

</xml_diff>